<commit_message>
Adds PCB component population details and links to 3D models
Sets 'populate' attribute to 'no' for specific resistors in different variants.
Enables linking of PCB layout to 3D model view.
Incorporates a new variant definition in both schematic and board files.

Removes outdated CPL file and updates BOM Excel file.
</commit_message>
<xml_diff>
--- a/Hutschienenmoped-XL/Sample-BOM_JLCSMT.xlsx
+++ b/Hutschienenmoped-XL/Sample-BOM_JLCSMT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ms\ISOBUS_Hardware\Hutschienenmoped-XL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054761BC-B78B-41ED-AD1B-0AE1483945F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C261DB7-6321-439F-994D-8463B4A4A59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42225" yWindow="1485" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5535" yWindow="1155" windowWidth="28800" windowHeight="19140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="108">
   <si>
     <t>Comment</t>
   </si>
@@ -69,13 +69,202 @@
     </r>
   </si>
   <si>
+    <t>638207222005</t>
+  </si>
+  <si>
+    <t>638207222007</t>
+  </si>
+  <si>
+    <t>638207222008</t>
+  </si>
+  <si>
+    <t>0R</t>
+  </si>
+  <si>
+    <t>1 nF</t>
+  </si>
+  <si>
+    <t>100 nF</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>13K</t>
+  </si>
+  <si>
+    <t>150141VS73100</t>
+  </si>
+  <si>
+    <t>1k2</t>
+  </si>
+  <si>
+    <t>22 µF</t>
+  </si>
+  <si>
+    <t>22K</t>
+  </si>
+  <si>
+    <t>24Vdc</t>
+  </si>
+  <si>
+    <t>33 nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">330  µF </t>
+  </si>
+  <si>
+    <t>33V</t>
+  </si>
+  <si>
+    <t>47 nF</t>
+  </si>
+  <si>
+    <t>470Ohm</t>
+  </si>
+  <si>
+    <t>47K</t>
+  </si>
+  <si>
+    <t>47R</t>
+  </si>
+  <si>
+    <t>4k7</t>
+  </si>
+  <si>
+    <t>510R</t>
+  </si>
+  <si>
+    <t>60R</t>
+  </si>
+  <si>
+    <t>61300421121</t>
+  </si>
+  <si>
+    <t>61302211821</t>
+  </si>
+  <si>
+    <t>62100421021</t>
+  </si>
+  <si>
+    <t>645004114822</t>
+  </si>
+  <si>
+    <t>820R</t>
+  </si>
+  <si>
+    <t>BAS70-04</t>
+  </si>
+  <si>
+    <t>BTM9010EP</t>
+  </si>
+  <si>
+    <t>DMT6007LFG-7</t>
+  </si>
+  <si>
+    <t>EDZVT2R3.3B</t>
+  </si>
+  <si>
+    <t>GS1J-L</t>
+  </si>
+  <si>
+    <t>LM74700QDBVTQ1</t>
+  </si>
+  <si>
+    <t>MBRS340T3</t>
+  </si>
+  <si>
+    <t>NCV1117DT50RKG</t>
+  </si>
+  <si>
+    <t>SMD3216-090N</t>
+  </si>
+  <si>
+    <t>TLE9250VSJ</t>
+  </si>
+  <si>
+    <t>RESET</t>
+  </si>
+  <si>
     <t>J5, J9</t>
   </si>
   <si>
-    <t>U2, U3, U5, U6</t>
-  </si>
-  <si>
-    <t>G1</t>
+    <t>U2, U3</t>
+  </si>
+  <si>
+    <t>J1, J7, J13</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>J15</t>
+  </si>
+  <si>
+    <t>R62, R63</t>
+  </si>
+  <si>
+    <t>C13, C20</t>
+  </si>
+  <si>
+    <t>C11, C26, C27, C28, C32, C34, C40, C42, C48, C50</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C5, C6, C17, C18, C19, C35, C36</t>
+  </si>
+  <si>
+    <t>R14, R15, R16, R17, R19, R20, R33, R34</t>
+  </si>
+  <si>
+    <t>D1, D2, D3, D4, D7, D8, D9, D10</t>
+  </si>
+  <si>
+    <t>R35, R36</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>R23, R26, R31, R32, R41, R44, R53, R56</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>C4, C7, C8, C9, C14, C16, C21, C22, C24, C25, C31, C33, C39, C41, C47, C49</t>
+  </si>
+  <si>
+    <t>C23</t>
+  </si>
+  <si>
+    <t>C29, C30</t>
+  </si>
+  <si>
+    <t>D0, D5</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>RX1, RX2, RX3, RX4, RX5, RX6, RX7, RX8</t>
+  </si>
+  <si>
+    <t>R22, R25, R29, R30, R40, R43, R52, R55</t>
+  </si>
+  <si>
+    <t>R7, R10</t>
+  </si>
+  <si>
+    <t>R2, R4, R5, R6, R9, R11, R13, R18, R37, R38</t>
+  </si>
+  <si>
+    <t>R45, R46, R47, R48, R49, R50, R57, R58</t>
+  </si>
+  <si>
+    <t>R1, R3</t>
   </si>
   <si>
     <t>J4</t>
@@ -84,229 +273,112 @@
     <t>ESP32-J1, ESP32-J3</t>
   </si>
   <si>
-    <t>J1, J7, J13</t>
-  </si>
-  <si>
-    <t>J8</t>
-  </si>
-  <si>
-    <t>J15</t>
-  </si>
-  <si>
-    <t>C1, C2, C3, C5, C6, C13, C17, C18, C19, C20</t>
-  </si>
-  <si>
-    <t>C24, C25, C26, C27, C31, C32, C33, C34, C39, C40, C41, C42, C47, C48, C49, C50</t>
-  </si>
-  <si>
-    <t>C4, C7, C8, C9, C14, C16, C21, C22</t>
-  </si>
-  <si>
-    <t>D1, D2, D3, D4, D7, D8, D9, D10</t>
+    <t>J3, J6, J10, J11</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>R8, R12</t>
+  </si>
+  <si>
+    <t>D012, D015, D024, D026, D028, D030, D032, D034</t>
+  </si>
+  <si>
+    <t>U1, U5</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>D013, D017, D025, D027, D029, D031, D033, D035</t>
+  </si>
+  <si>
+    <t>D014, D016, D018, D019, D020, D021, D022, D023</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>D006</t>
+  </si>
+  <si>
+    <t>IC2</t>
+  </si>
+  <si>
+    <t>U6, U8, U9, U10, U11, U12, U13, U14</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>4312560837X6</t>
+  </si>
+  <si>
+    <t>SOP65P600X115-15N-V</t>
+  </si>
+  <si>
+    <t>RESC1608X60</t>
+  </si>
+  <si>
+    <t>WCAP-CSGP_0603_H0.8_R</t>
+  </si>
+  <si>
+    <t>WL-SMTW_3528</t>
+  </si>
+  <si>
+    <t>RESC1005X40</t>
+  </si>
+  <si>
+    <t>WCAP-CSGP_0805_H1.25_R</t>
+  </si>
+  <si>
+    <t>WCAP-CSGP_1210_H2.5</t>
+  </si>
+  <si>
+    <t>WE-TVS_SOT23-3L</t>
+  </si>
+  <si>
+    <t>WCAP-ASLI_12.5X14(DXL)</t>
+  </si>
+  <si>
+    <t>WCAP-ASLI_8X10.5(DXL)</t>
+  </si>
+  <si>
+    <t>WE-TVSP_DO-214AB_BIDIRECTIONAL</t>
+  </si>
+  <si>
+    <t>RESC3216X70</t>
+  </si>
+  <si>
+    <t>RESC2012X65</t>
+  </si>
+  <si>
+    <t>SOT23</t>
+  </si>
+  <si>
+    <t>DMP4013LFG7</t>
+  </si>
+  <si>
+    <t>SODFL1608X70N</t>
+  </si>
+  <si>
+    <t>DIOM5226X290N</t>
+  </si>
+  <si>
+    <t>SOT95P280X145-6N</t>
+  </si>
+  <si>
+    <t>SMC</t>
+  </si>
+  <si>
+    <t>SOIC127P602X173-8N-V</t>
+  </si>
+  <si>
+    <t>61300621121</t>
   </si>
   <si>
     <t>R21, R24, R27, R28, R39, R42, R51, R54</t>
-  </si>
-  <si>
-    <t>C12</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>D11</t>
-  </si>
-  <si>
-    <t>D12, D13, D15, D17</t>
-  </si>
-  <si>
-    <t>C23</t>
-  </si>
-  <si>
-    <t>D0, D5</t>
-  </si>
-  <si>
-    <t>RX1, RX2, RX3, RX4, RX5, RX6, RX7, RX8</t>
-  </si>
-  <si>
-    <t>R22, R25, R29, R30, R40, R43, R52, R55</t>
-  </si>
-  <si>
-    <t>R7, R8, R10, R12</t>
-  </si>
-  <si>
-    <t>C15</t>
-  </si>
-  <si>
-    <t>R2, R4, R5, R6, R9, R11, R13, R18</t>
-  </si>
-  <si>
-    <t>R1, R3</t>
-  </si>
-  <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t>D006</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>SOP65P600X115-15N-V</t>
-  </si>
-  <si>
-    <t>INF-PG-TO252-3-11_N</t>
-  </si>
-  <si>
-    <t>WCAP-CSGP_0805_H0.8_R</t>
-  </si>
-  <si>
-    <t>WCAP-CSGP_1206_H0.8</t>
-  </si>
-  <si>
-    <t>R1206</t>
-  </si>
-  <si>
-    <t>WL-SMTW_3528</t>
-  </si>
-  <si>
-    <t>WCAP-CSGP_0805_H1.25_R</t>
-  </si>
-  <si>
-    <t>WCAP-CSGP_1210_H2.5</t>
-  </si>
-  <si>
-    <t>WE-TVS_SOT23-3L</t>
-  </si>
-  <si>
-    <t>WE-TVS_SOT143-4L</t>
-  </si>
-  <si>
-    <t>WCAP-ASLI_12.5X14(DXL)</t>
-  </si>
-  <si>
-    <t>WE-TVSP_DO-214AB_BIDIRECTIONAL</t>
-  </si>
-  <si>
-    <t>R0805</t>
-  </si>
-  <si>
-    <t>SMC</t>
-  </si>
-  <si>
-    <t>SOIC127P602X173-8N-V</t>
-  </si>
-  <si>
-    <t>61300621121</t>
-  </si>
-  <si>
-    <t>61300421121</t>
-  </si>
-  <si>
-    <t>61302211821</t>
-  </si>
-  <si>
-    <t>638207222005</t>
-  </si>
-  <si>
-    <t>638207222007</t>
-  </si>
-  <si>
-    <t>638207222008</t>
-  </si>
-  <si>
-    <t>645004114822</t>
-  </si>
-  <si>
-    <t>100nF</t>
-  </si>
-  <si>
-    <t>10nF</t>
-  </si>
-  <si>
-    <t>13K</t>
-  </si>
-  <si>
-    <t>150141VS73100</t>
-  </si>
-  <si>
-    <t>1K2</t>
-  </si>
-  <si>
-    <t>22uF</t>
-  </si>
-  <si>
-    <t>24Vdc</t>
-  </si>
-  <si>
-    <t>3.3Vdc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">330  ÂµF </t>
-  </si>
-  <si>
-    <t>33V</t>
-  </si>
-  <si>
-    <t>470Ohm</t>
-  </si>
-  <si>
-    <t>47K</t>
-  </si>
-  <si>
-    <t>47R</t>
-  </si>
-  <si>
-    <t>47nF</t>
-  </si>
-  <si>
-    <t>4k7</t>
-  </si>
-  <si>
-    <t>60R</t>
-  </si>
-  <si>
-    <t>MBRS340T3</t>
-  </si>
-  <si>
-    <t>TLE9250VSJ</t>
-  </si>
-  <si>
-    <t>RESET</t>
-  </si>
-  <si>
-    <t>R14, R15, R16, R17, R19, R20, R23, R26, R31, R32, R33, R34, R41, R44, R53, R56</t>
-  </si>
-  <si>
-    <t>R35, R36, R37, R38</t>
-  </si>
-  <si>
-    <t>D014, D016, D018, D019, D020, D021, D022, D023</t>
-  </si>
-  <si>
-    <t>1k2</t>
-  </si>
-  <si>
-    <t>GS1J-L</t>
-  </si>
-  <si>
-    <t>431256083736</t>
-  </si>
-  <si>
-    <t>6130XX21121_61300621121</t>
-  </si>
-  <si>
-    <t>BTS7030-2EPA</t>
-  </si>
-  <si>
-    <t>IFX27001TF_V50</t>
-  </si>
-  <si>
-    <t>4312560837X6</t>
-  </si>
-  <si>
-    <t>SMA_DO-214AC</t>
   </si>
 </sst>
 </file>
@@ -747,16 +819,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="26" style="2" customWidth="1"/>
-    <col min="2" max="2" width="80.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" customWidth="1"/>
     <col min="3" max="3" width="36.125" customWidth="1"/>
     <col min="4" max="4" width="24.5" customWidth="1"/>
   </cols>
@@ -776,362 +848,488 @@
       </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="7" t="s">
-        <v>78</v>
-      </c>
+      <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="6" t="s">
-        <v>79</v>
-      </c>
+      <c r="A3" s="6"/>
       <c r="B3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="6" t="s">
-        <v>81</v>
-      </c>
       <c r="B5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>33</v>
+        <v>45</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="7" t="s">
+      <c r="C9" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>52</v>
+      <c r="C10" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="6" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="6" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="6" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="6" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="6" t="s">
-        <v>76</v>
+        <v>14</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="6" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="6" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="6" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="6" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="6" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="6" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="6" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="6" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="6" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A30" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="C30" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A31" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A32" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A30" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="6" t="s">
+      <c r="B32" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A33" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A31" s="6" t="s">
+      <c r="B33" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A34" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A35" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A36" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A37" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A38" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="6" t="s">
+      <c r="C38" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A39" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A40" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A41" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A42" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A43" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A44" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A32" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A33" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>46</v>
+      <c r="C44" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A45" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>